<commit_message>
imported google fonts, and icons as well
</commit_message>
<xml_diff>
--- a/ProjectInfo/Project-YoProgramo-PortfolioWeb-FullStack-Bravard-Manuel.xlsx
+++ b/ProjectInfo/Project-YoProgramo-PortfolioWeb-FullStack-Bravard-Manuel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03753a6eec3bd540/Documents/WEBMASTER/ArgPrograma/argentina programa - modulos - pdf/yoProgramo/desafios/modulo1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03753a6eec3bd540/Documents/WEBMASTER/ArgPrograma/Portfolio-YoProgramo-MaquetadoFront/ProjectInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1668" documentId="11_F25DC773A252ABDACC10489049DE7BF65BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77E723A3-5551-47EE-8FDE-8021532934A1}"/>
+  <xr:revisionPtr revIDLastSave="1683" documentId="11_F25DC773A252ABDACC10489049DE7BF65BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFDC5FD-9F06-46A2-B3F8-A45B9209CB00}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,21 +186,6 @@
     <t>Entorno PREprod</t>
   </si>
   <si>
-    <t>L - 14/11</t>
-  </si>
-  <si>
-    <t>M - 15/11</t>
-  </si>
-  <si>
-    <t>M - 16/11</t>
-  </si>
-  <si>
-    <t>J - 17/11</t>
-  </si>
-  <si>
-    <t>V - 18/11</t>
-  </si>
-  <si>
     <t>User Stories</t>
   </si>
   <si>
@@ -450,18 +435,12 @@
     <t>M - 23/11</t>
   </si>
   <si>
-    <t>J - 24/11</t>
-  </si>
-  <si>
     <t>V - 25/11</t>
   </si>
   <si>
     <t>L - 28/11</t>
   </si>
   <si>
-    <t>14/11-25/11</t>
-  </si>
-  <si>
     <t>Pendientes:</t>
   </si>
   <si>
@@ -547,6 +526,27 @@
   </si>
   <si>
     <t>EST. Total Hrs.:</t>
+  </si>
+  <si>
+    <t>21/11-02/12</t>
+  </si>
+  <si>
+    <t>J -24/11</t>
+  </si>
+  <si>
+    <t>M - 29/11</t>
+  </si>
+  <si>
+    <t>M - 30/11</t>
+  </si>
+  <si>
+    <t>L - 05/12</t>
+  </si>
+  <si>
+    <t>V - 02/12</t>
+  </si>
+  <si>
+    <t>J - 01/12</t>
   </si>
 </sst>
 </file>
@@ -1650,6 +1650,87 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1722,88 +1803,7 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1872,6 +1872,141 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1898,141 +2033,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2742,10 +2742,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3039,82 +3035,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="148"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="149"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="176"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="138" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="140"/>
+      <c r="O1" s="165" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="167"/>
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="150"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="152"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="179"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="176" t="s">
-        <v>150</v>
-      </c>
-      <c r="P2" s="177"/>
-      <c r="Q2" s="177"/>
-      <c r="R2" s="177"/>
-      <c r="S2" s="177"/>
-      <c r="T2" s="178"/>
+      <c r="O2" s="148" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="149"/>
+      <c r="R2" s="149"/>
+      <c r="S2" s="149"/>
+      <c r="T2" s="150"/>
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="180" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="154"/>
-      <c r="C3" s="155" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="157"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="182" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="183"/>
+      <c r="L3" s="183"/>
+      <c r="M3" s="184"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="176"/>
-      <c r="P3" s="177"/>
-      <c r="Q3" s="177"/>
-      <c r="R3" s="177"/>
-      <c r="S3" s="177"/>
-      <c r="T3" s="178"/>
+      <c r="O3" s="148"/>
+      <c r="P3" s="149"/>
+      <c r="Q3" s="149"/>
+      <c r="R3" s="149"/>
+      <c r="S3" s="149"/>
+      <c r="T3" s="150"/>
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3132,57 +3128,57 @@
       <c r="L4" s="92"/>
       <c r="M4" s="93"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="176"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="177"/>
-      <c r="S4" s="177"/>
-      <c r="T4" s="178"/>
+      <c r="O4" s="148"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
+      <c r="R4" s="149"/>
+      <c r="S4" s="149"/>
+      <c r="T4" s="150"/>
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="168" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="142"/>
-      <c r="D5" s="142"/>
-      <c r="E5" s="142"/>
-      <c r="F5" s="142"/>
-      <c r="G5" s="142"/>
-      <c r="H5" s="142"/>
-      <c r="I5" s="142"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="142"/>
-      <c r="L5" s="142"/>
-      <c r="M5" s="143"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="169"/>
+      <c r="H5" s="169"/>
+      <c r="I5" s="169"/>
+      <c r="J5" s="169"/>
+      <c r="K5" s="169"/>
+      <c r="L5" s="169"/>
+      <c r="M5" s="170"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="180"/>
-      <c r="Q5" s="180"/>
-      <c r="R5" s="180"/>
-      <c r="S5" s="180"/>
-      <c r="T5" s="181"/>
+      <c r="O5" s="151"/>
+      <c r="P5" s="152"/>
+      <c r="Q5" s="152"/>
+      <c r="R5" s="152"/>
+      <c r="S5" s="152"/>
+      <c r="T5" s="153"/>
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="89"/>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="171" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="145"/>
-      <c r="L6" s="145"/>
-      <c r="M6" s="146"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="172"/>
+      <c r="H6" s="172"/>
+      <c r="I6" s="172"/>
+      <c r="J6" s="172"/>
+      <c r="K6" s="172"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="173"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -3216,27 +3212,27 @@
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="158" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" s="159"/>
-      <c r="C8" s="160" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="161"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="158" t="s">
-        <v>132</v>
-      </c>
-      <c r="G8" s="163"/>
-      <c r="H8" s="163"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="160">
+      <c r="A8" s="185" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="186"/>
+      <c r="C8" s="156" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="157"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="185" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="187"/>
+      <c r="H8" s="187"/>
+      <c r="I8" s="186"/>
+      <c r="J8" s="156">
         <v>7</v>
       </c>
-      <c r="K8" s="161"/>
-      <c r="L8" s="161"/>
-      <c r="M8" s="162"/>
+      <c r="K8" s="157"/>
+      <c r="L8" s="157"/>
+      <c r="M8" s="158"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -3270,25 +3266,25 @@
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="136" t="s">
+      <c r="A10" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="137"/>
+      <c r="B10" s="164"/>
       <c r="C10" s="106"/>
       <c r="D10" s="103" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="94"/>
       <c r="F10" s="106"/>
-      <c r="G10" s="184" t="s">
+      <c r="G10" s="159" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="184"/>
-      <c r="I10" s="185"/>
+      <c r="H10" s="159"/>
+      <c r="I10" s="160"/>
       <c r="J10" s="109"/>
-      <c r="K10" s="182"/>
-      <c r="L10" s="182"/>
-      <c r="M10" s="183"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="154"/>
+      <c r="M10" s="155"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -3301,7 +3297,7 @@
     <row r="11" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
       <c r="B11" s="97" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C11" s="107"/>
       <c r="D11" s="104" t="s">
@@ -3309,15 +3305,15 @@
       </c>
       <c r="E11" s="95"/>
       <c r="F11" s="107"/>
-      <c r="G11" s="186" t="s">
+      <c r="G11" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="186"/>
-      <c r="I11" s="187"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="162"/>
       <c r="J11" s="101"/>
-      <c r="K11" s="182"/>
-      <c r="L11" s="182"/>
-      <c r="M11" s="183"/>
+      <c r="K11" s="154"/>
+      <c r="L11" s="154"/>
+      <c r="M11" s="155"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -3330,7 +3326,7 @@
     <row r="12" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="101"/>
       <c r="B12" s="98" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C12" s="107"/>
       <c r="D12" s="104" t="s">
@@ -3338,15 +3334,15 @@
       </c>
       <c r="E12" s="95"/>
       <c r="F12" s="107"/>
-      <c r="G12" s="186" t="s">
+      <c r="G12" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="186"/>
-      <c r="I12" s="187"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="162"/>
       <c r="J12" s="101"/>
-      <c r="K12" s="182"/>
-      <c r="L12" s="182"/>
-      <c r="M12" s="183"/>
+      <c r="K12" s="154"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="155"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -3359,7 +3355,7 @@
     <row r="13" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="102"/>
       <c r="B13" s="99" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="107"/>
       <c r="D13" s="104" t="s">
@@ -3367,13 +3363,13 @@
       </c>
       <c r="E13" s="95"/>
       <c r="F13" s="107"/>
-      <c r="G13" s="182"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="183"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="155"/>
       <c r="J13" s="101"/>
-      <c r="K13" s="182"/>
-      <c r="L13" s="182"/>
-      <c r="M13" s="183"/>
+      <c r="K13" s="154"/>
+      <c r="L13" s="154"/>
+      <c r="M13" s="155"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -3392,13 +3388,13 @@
       </c>
       <c r="E14" s="95"/>
       <c r="F14" s="107"/>
-      <c r="G14" s="182"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="183"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="155"/>
       <c r="J14" s="101"/>
-      <c r="K14" s="182"/>
-      <c r="L14" s="182"/>
-      <c r="M14" s="183"/>
+      <c r="K14" s="154"/>
+      <c r="L14" s="154"/>
+      <c r="M14" s="155"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -3417,13 +3413,13 @@
       </c>
       <c r="E15" s="96"/>
       <c r="F15" s="108"/>
-      <c r="G15" s="182"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="183"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="155"/>
       <c r="J15" s="102"/>
-      <c r="K15" s="182"/>
-      <c r="L15" s="182"/>
-      <c r="M15" s="183"/>
+      <c r="K15" s="154"/>
+      <c r="L15" s="154"/>
+      <c r="M15" s="155"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -3480,19 +3476,19 @@
       <c r="U17" s="1"/>
     </row>
     <row r="18" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="173" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="164" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="165"/>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="166"/>
+      <c r="A18" s="145" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="136" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="138"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -3507,15 +3503,15 @@
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="174"/>
-      <c r="B19" s="167"/>
-      <c r="C19" s="168"/>
-      <c r="D19" s="168"/>
-      <c r="E19" s="168"/>
-      <c r="F19" s="168"/>
-      <c r="G19" s="168"/>
-      <c r="H19" s="168"/>
-      <c r="I19" s="169"/>
+      <c r="A19" s="146"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="140"/>
+      <c r="I19" s="141"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -3530,15 +3526,15 @@
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="1:21" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="175"/>
-      <c r="B20" s="170"/>
-      <c r="C20" s="171"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="171"/>
-      <c r="F20" s="171"/>
-      <c r="G20" s="171"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="172"/>
+      <c r="A20" s="147"/>
+      <c r="B20" s="142"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="143"/>
+      <c r="E20" s="143"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="143"/>
+      <c r="I20" s="144"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -3581,6 +3577,16 @@
     <row r="30" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="A1:M2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
     <mergeCell ref="B18:I20"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="O2:T5"/>
@@ -3597,16 +3603,6 @@
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="A1:M2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3700,7 +3696,7 @@
     </row>
     <row r="4" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="208" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B4" s="209"/>
       <c r="C4" s="113"/>
@@ -3748,7 +3744,7 @@
     </row>
     <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="122" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B6" s="111"/>
       <c r="C6" s="111"/>
@@ -3773,7 +3769,7 @@
     </row>
     <row r="7" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="116" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" s="113"/>
       <c r="C7" s="113"/>
@@ -3821,7 +3817,7 @@
     </row>
     <row r="9" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="116" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B9" s="113"/>
       <c r="C9" s="113"/>
@@ -3869,7 +3865,7 @@
     </row>
     <row r="11" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="116" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B11" s="113"/>
       <c r="C11" s="113"/>
@@ -3894,7 +3890,7 @@
     </row>
     <row r="12" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="123" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B12" s="119"/>
       <c r="C12" s="119"/>
@@ -3965,7 +3961,7 @@
     </row>
     <row r="15" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="206" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B15" s="207"/>
       <c r="C15" s="113"/>
@@ -4013,7 +4009,7 @@
     </row>
     <row r="17" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="124" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B17" s="111"/>
       <c r="C17" s="111"/>
@@ -4038,7 +4034,7 @@
     </row>
     <row r="18" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="116" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="113"/>
       <c r="C18" s="113"/>
@@ -4063,7 +4059,7 @@
     </row>
     <row r="19" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="116" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B19" s="113"/>
       <c r="C19" s="113"/>
@@ -4111,7 +4107,7 @@
     </row>
     <row r="21" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" s="118" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B21" s="113"/>
       <c r="C21" s="113"/>
@@ -4136,7 +4132,7 @@
     </row>
     <row r="22" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="116" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B22" s="113"/>
       <c r="C22" s="113"/>
@@ -4184,7 +4180,7 @@
     </row>
     <row r="24" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="118" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B24" s="113"/>
       <c r="C24" s="113"/>
@@ -4209,7 +4205,7 @@
     </row>
     <row r="25" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="123" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B25" s="119"/>
       <c r="C25" s="119"/>
@@ -4280,7 +4276,7 @@
     </row>
     <row r="28" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="206" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B28" s="207"/>
       <c r="C28" s="113"/>
@@ -4328,7 +4324,7 @@
     </row>
     <row r="30" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="121" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B30" s="113"/>
       <c r="C30" s="113"/>
@@ -4376,7 +4372,7 @@
     </row>
     <row r="32" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="122" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B32" s="111"/>
       <c r="C32" s="111"/>
@@ -4401,7 +4397,7 @@
     </row>
     <row r="33" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="116" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B33" s="113"/>
       <c r="C33" s="113"/>
@@ -4449,7 +4445,7 @@
     </row>
     <row r="35" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="116" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B35" s="113"/>
       <c r="C35" s="113"/>
@@ -4497,7 +4493,7 @@
     </row>
     <row r="37" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="116" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B37" s="113"/>
       <c r="C37" s="113"/>
@@ -4522,7 +4518,7 @@
     </row>
     <row r="38" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="116" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B38" s="113"/>
       <c r="C38" s="113"/>
@@ -4570,7 +4566,7 @@
     </row>
     <row r="40" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="116" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B40" s="113"/>
       <c r="C40" s="113"/>
@@ -4618,7 +4614,7 @@
     </row>
     <row r="42" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="116" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B42" s="113"/>
       <c r="C42" s="113"/>
@@ -4666,7 +4662,7 @@
     </row>
     <row r="44" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="116" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B44" s="113"/>
       <c r="C44" s="113"/>
@@ -4714,7 +4710,7 @@
     </row>
     <row r="46" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" s="121" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B46" s="113"/>
       <c r="C46" s="113"/>
@@ -4762,7 +4758,7 @@
     </row>
     <row r="48" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="122" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B48" s="111"/>
       <c r="C48" s="111"/>
@@ -4810,7 +4806,7 @@
     </row>
     <row r="50" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="116" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B50" s="113"/>
       <c r="C50" s="113"/>
@@ -4858,7 +4854,7 @@
     </row>
     <row r="52" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="116" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B52" s="113"/>
       <c r="C52" s="113"/>
@@ -4906,7 +4902,7 @@
     </row>
     <row r="54" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="123" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B54" s="119"/>
       <c r="C54" s="119"/>
@@ -4954,7 +4950,7 @@
     </row>
     <row r="56" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" s="121" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B56" s="113"/>
       <c r="C56" s="113"/>
@@ -5002,7 +4998,7 @@
     </row>
     <row r="58" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="122" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B58" s="111"/>
       <c r="C58" s="111"/>
@@ -5050,7 +5046,7 @@
     </row>
     <row r="60" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="116" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B60" s="113"/>
       <c r="C60" s="113"/>
@@ -5098,7 +5094,7 @@
     </row>
     <row r="62" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="116" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B62" s="113"/>
       <c r="C62" s="113"/>
@@ -5123,7 +5119,7 @@
     </row>
     <row r="63" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="123" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B63" s="119"/>
       <c r="C63" s="119"/>
@@ -5171,7 +5167,7 @@
     </row>
     <row r="65" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" s="121" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B65" s="113"/>
       <c r="C65" s="113"/>
@@ -5219,7 +5215,7 @@
     </row>
     <row r="67" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="127" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B67" s="128"/>
       <c r="C67" s="128"/>
@@ -5336,7 +5332,7 @@
     </row>
     <row r="72" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A72" s="203" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B72" s="205"/>
       <c r="C72" s="113"/>
@@ -5361,7 +5357,7 @@
     </row>
     <row r="73" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="203" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B73" s="204"/>
       <c r="C73" s="204"/>
@@ -5386,10 +5382,10 @@
     </row>
     <row r="74" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="130" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B74" s="200" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C74" s="201"/>
       <c r="D74" s="201"/>
@@ -5413,10 +5409,10 @@
     </row>
     <row r="75" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="131" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B75" s="197" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C75" s="198"/>
       <c r="D75" s="198"/>
@@ -5440,10 +5436,10 @@
     </row>
     <row r="76" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="131" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B76" s="188" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C76" s="189"/>
       <c r="D76" s="189"/>
@@ -5467,11 +5463,11 @@
     </row>
     <row r="77" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="131" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B77" s="131"/>
       <c r="C77" s="135" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D77" s="132"/>
       <c r="E77" s="133"/>
@@ -5484,12 +5480,12 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
@@ -5528,8 +5524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9294F5ED-0613-4755-9735-C7266C041EF2}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5541,43 +5537,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="210" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="241"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="211"/>
+      <c r="K1" s="212"/>
     </row>
     <row r="2" spans="1:11" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="242"/>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243"/>
-      <c r="H2" s="243"/>
-      <c r="I2" s="243"/>
-      <c r="J2" s="243"/>
-      <c r="K2" s="244"/>
+      <c r="A2" s="213"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214"/>
+      <c r="J2" s="214"/>
+      <c r="K2" s="215"/>
     </row>
     <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A3" s="226" t="s">
+      <c r="A3" s="242" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="226"/>
+      <c r="B3" s="242"/>
+      <c r="C3" s="242"/>
+      <c r="D3" s="242" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="242"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -5599,70 +5595,70 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="257" t="s">
+      <c r="A5" s="228" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="258"/>
-      <c r="C5" s="258"/>
-      <c r="D5" s="258"/>
-      <c r="E5" s="258"/>
-      <c r="F5" s="258"/>
-      <c r="G5" s="258"/>
-      <c r="H5" s="258"/>
-      <c r="I5" s="258"/>
-      <c r="J5" s="258"/>
-      <c r="K5" s="259"/>
+      <c r="B5" s="229"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
+      <c r="G5" s="229"/>
+      <c r="H5" s="229"/>
+      <c r="I5" s="229"/>
+      <c r="J5" s="229"/>
+      <c r="K5" s="230"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="231" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="261"/>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="262"/>
+      <c r="B6" s="232"/>
+      <c r="C6" s="232"/>
+      <c r="D6" s="232"/>
+      <c r="E6" s="232"/>
+      <c r="F6" s="232"/>
+      <c r="G6" s="232"/>
+      <c r="H6" s="232"/>
+      <c r="I6" s="232"/>
+      <c r="J6" s="233"/>
       <c r="K6" s="45" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="H7" s="47" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="J7" s="47" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="K7" s="48" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -5701,7 +5697,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="263" t="s">
+      <c r="A9" s="234" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="235" t="s">
@@ -5728,15 +5724,15 @@
       <c r="I9" s="235" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="225" t="s">
+      <c r="J9" s="237" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="236" t="s">
+      <c r="K9" s="238" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="263"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="235"/>
       <c r="C10" s="235"/>
       <c r="D10" s="235"/>
@@ -5745,11 +5741,11 @@
       <c r="G10" s="235"/>
       <c r="H10" s="235"/>
       <c r="I10" s="235"/>
-      <c r="J10" s="225"/>
-      <c r="K10" s="236"/>
+      <c r="J10" s="237"/>
+      <c r="K10" s="238"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="263"/>
+      <c r="A11" s="234"/>
       <c r="B11" s="235"/>
       <c r="C11" s="235"/>
       <c r="D11" s="235"/>
@@ -5758,11 +5754,11 @@
       <c r="G11" s="235"/>
       <c r="H11" s="235"/>
       <c r="I11" s="235"/>
-      <c r="J11" s="225"/>
-      <c r="K11" s="236"/>
+      <c r="J11" s="237"/>
+      <c r="K11" s="238"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="263"/>
+      <c r="A12" s="234"/>
       <c r="B12" s="235"/>
       <c r="C12" s="235"/>
       <c r="D12" s="235"/>
@@ -5771,13 +5767,13 @@
       <c r="G12" s="235"/>
       <c r="H12" s="235"/>
       <c r="I12" s="235"/>
-      <c r="J12" s="237" t="s">
+      <c r="J12" s="239" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="236"/>
+      <c r="K12" s="238"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="263"/>
+      <c r="A13" s="234"/>
       <c r="B13" s="235"/>
       <c r="C13" s="235"/>
       <c r="D13" s="235"/>
@@ -5786,11 +5782,11 @@
       <c r="G13" s="235"/>
       <c r="H13" s="235"/>
       <c r="I13" s="235"/>
-      <c r="J13" s="237"/>
-      <c r="K13" s="236"/>
+      <c r="J13" s="239"/>
+      <c r="K13" s="238"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="263"/>
+      <c r="A14" s="234"/>
       <c r="B14" s="235"/>
       <c r="C14" s="235"/>
       <c r="D14" s="235"/>
@@ -5799,11 +5795,11 @@
       <c r="G14" s="235"/>
       <c r="H14" s="235"/>
       <c r="I14" s="235"/>
-      <c r="J14" s="237"/>
-      <c r="K14" s="236"/>
+      <c r="J14" s="239"/>
+      <c r="K14" s="238"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="240" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="235"/>
@@ -5813,14 +5809,14 @@
       <c r="F15" s="235"/>
       <c r="G15" s="235"/>
       <c r="H15" s="235"/>
-      <c r="I15" s="225" t="s">
+      <c r="I15" s="237" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="237"/>
-      <c r="K15" s="236"/>
+      <c r="J15" s="239"/>
+      <c r="K15" s="238"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="223"/>
+      <c r="A16" s="240"/>
       <c r="B16" s="235"/>
       <c r="C16" s="235"/>
       <c r="D16" s="235"/>
@@ -5828,14 +5824,14 @@
       <c r="F16" s="235"/>
       <c r="G16" s="235"/>
       <c r="H16" s="235"/>
-      <c r="I16" s="225"/>
-      <c r="J16" s="237"/>
-      <c r="K16" s="255" t="s">
+      <c r="I16" s="237"/>
+      <c r="J16" s="239"/>
+      <c r="K16" s="226" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="223"/>
+      <c r="A17" s="240"/>
       <c r="B17" s="235"/>
       <c r="C17" s="235"/>
       <c r="D17" s="235"/>
@@ -5843,14 +5839,14 @@
       <c r="F17" s="235"/>
       <c r="G17" s="235"/>
       <c r="H17" s="235"/>
-      <c r="I17" s="225"/>
-      <c r="J17" s="256" t="s">
+      <c r="I17" s="237"/>
+      <c r="J17" s="227" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="255"/>
+      <c r="K17" s="226"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="223"/>
+      <c r="A18" s="240"/>
       <c r="B18" s="235"/>
       <c r="C18" s="235"/>
       <c r="D18" s="235"/>
@@ -5858,12 +5854,12 @@
       <c r="F18" s="235"/>
       <c r="G18" s="235"/>
       <c r="H18" s="235"/>
-      <c r="I18" s="225"/>
-      <c r="J18" s="256"/>
-      <c r="K18" s="255"/>
+      <c r="I18" s="237"/>
+      <c r="J18" s="227"/>
+      <c r="K18" s="226"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="223"/>
+      <c r="A19" s="240"/>
       <c r="B19" s="235"/>
       <c r="C19" s="235"/>
       <c r="D19" s="235"/>
@@ -5871,26 +5867,26 @@
       <c r="F19" s="235"/>
       <c r="G19" s="235"/>
       <c r="H19" s="235"/>
-      <c r="I19" s="225"/>
-      <c r="J19" s="256"/>
-      <c r="K19" s="255"/>
+      <c r="I19" s="237"/>
+      <c r="J19" s="227"/>
+      <c r="K19" s="226"/>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="224"/>
-      <c r="B20" s="238"/>
-      <c r="C20" s="238"/>
-      <c r="D20" s="238"/>
-      <c r="E20" s="238"/>
-      <c r="F20" s="238"/>
+      <c r="A20" s="241"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
+      <c r="E20" s="236"/>
+      <c r="F20" s="236"/>
       <c r="G20" s="235"/>
       <c r="H20" s="235"/>
-      <c r="I20" s="225"/>
-      <c r="J20" s="256"/>
-      <c r="K20" s="255"/>
+      <c r="I20" s="237"/>
+      <c r="J20" s="227"/>
+      <c r="K20" s="226"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="55" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B21" s="56"/>
       <c r="C21" s="56"/>
@@ -5908,7 +5904,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="50">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>13</v>
@@ -5939,7 +5935,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E23" s="50">
         <f>K59+B24+B25+E22</f>
@@ -5965,14 +5961,14 @@
         <v>12</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E24" s="50">
         <f>J59</f>
         <v>8.25</v>
       </c>
       <c r="F24" s="58" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
@@ -6014,11 +6010,11 @@
     </row>
     <row r="27" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
@@ -6044,11 +6040,11 @@
     </row>
     <row r="29" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="31" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
@@ -6063,7 +6059,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="24" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="36"/>
@@ -6091,7 +6087,7 @@
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -6119,7 +6115,7 @@
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="24" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -6134,7 +6130,7 @@
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -6162,7 +6158,7 @@
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="24" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -6190,7 +6186,7 @@
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -6218,7 +6214,7 @@
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="25" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -6244,11 +6240,11 @@
     </row>
     <row r="43" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="31" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="1"/>
@@ -6274,11 +6270,11 @@
     </row>
     <row r="45" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B45" s="31"/>
       <c r="C45" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D45" s="27"/>
       <c r="E45" s="1"/>
@@ -6304,11 +6300,11 @@
     </row>
     <row r="47" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A47" s="31" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B47" s="31"/>
       <c r="C47" s="40" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D47" s="60"/>
       <c r="E47" s="21"/>
@@ -6323,7 +6319,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
@@ -6338,7 +6334,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -6353,7 +6349,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -6368,7 +6364,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
@@ -6383,7 +6379,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
@@ -6398,7 +6394,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -6413,7 +6409,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="43" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
@@ -6452,55 +6448,55 @@
     </row>
     <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="38"/>
-      <c r="B57" s="245" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="246"/>
-      <c r="D57" s="246"/>
-      <c r="E57" s="246"/>
-      <c r="F57" s="246"/>
-      <c r="G57" s="246"/>
-      <c r="H57" s="246"/>
-      <c r="I57" s="246"/>
-      <c r="J57" s="246"/>
-      <c r="K57" s="247"/>
+      <c r="B57" s="216" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="217"/>
+      <c r="D57" s="217"/>
+      <c r="E57" s="217"/>
+      <c r="F57" s="217"/>
+      <c r="G57" s="217"/>
+      <c r="H57" s="217"/>
+      <c r="I57" s="217"/>
+      <c r="J57" s="217"/>
+      <c r="K57" s="218"/>
     </row>
     <row r="58" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="39"/>
       <c r="B58" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="G58" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C58" s="61" t="s">
+      <c r="H58" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="F58" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="G58" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="H58" s="62" t="s">
-        <v>102</v>
-      </c>
       <c r="I58" s="63" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J58" s="64" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="K58" s="66" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="68" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B59" s="69">
         <v>0.5</v>
@@ -6536,111 +6532,111 @@
       </c>
     </row>
     <row r="60" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="252" t="s">
+      <c r="A60" s="223" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="248" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="219" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="232" t="s">
-        <v>104</v>
-      </c>
-      <c r="C60" s="248" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" s="248" t="s">
-        <v>110</v>
+      <c r="D60" s="219" t="s">
+        <v>105</v>
       </c>
       <c r="E60" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="F60" s="248" t="s">
-        <v>110</v>
-      </c>
-      <c r="G60" s="248" t="s">
-        <v>110</v>
-      </c>
-      <c r="H60" s="250" t="s">
-        <v>110</v>
-      </c>
-      <c r="I60" s="250" t="s">
-        <v>110</v>
+        <v>115</v>
+      </c>
+      <c r="F60" s="219" t="s">
+        <v>105</v>
+      </c>
+      <c r="G60" s="219" t="s">
+        <v>105</v>
+      </c>
+      <c r="H60" s="221" t="s">
+        <v>105</v>
+      </c>
+      <c r="I60" s="221" t="s">
+        <v>105</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="253"/>
-      <c r="B61" s="233"/>
-      <c r="C61" s="249"/>
-      <c r="D61" s="249"/>
+      <c r="A61" s="224"/>
+      <c r="B61" s="249"/>
+      <c r="C61" s="220"/>
+      <c r="D61" s="220"/>
       <c r="E61" s="72" t="s">
-        <v>122</v>
-      </c>
-      <c r="F61" s="249"/>
-      <c r="G61" s="249"/>
-      <c r="H61" s="251"/>
-      <c r="I61" s="251"/>
+        <v>117</v>
+      </c>
+      <c r="F61" s="220"/>
+      <c r="G61" s="220"/>
+      <c r="H61" s="222"/>
+      <c r="I61" s="222"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="253"/>
+      <c r="A62" s="224"/>
       <c r="B62" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="C62" s="249"/>
+        <v>100</v>
+      </c>
+      <c r="C62" s="220"/>
       <c r="D62" s="74" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E62" s="74" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F62" s="74" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G62" s="74" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H62" s="75" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I62" s="75" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="253"/>
+      <c r="A63" s="224"/>
       <c r="B63" s="73" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="249" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="C63" s="220" t="s">
+        <v>104</v>
       </c>
       <c r="D63" s="74" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E63" s="74"/>
       <c r="F63" s="74" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G63" s="74" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H63" s="74" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I63" s="75" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
     <row r="64" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="253"/>
-      <c r="B64" s="233" t="s">
-        <v>107</v>
-      </c>
-      <c r="C64" s="249"/>
+      <c r="A64" s="224"/>
+      <c r="B64" s="249" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="220"/>
       <c r="D64" s="74"/>
       <c r="E64" s="74"/>
       <c r="F64" s="74"/>
@@ -6651,8 +6647,8 @@
       <c r="K64" s="1"/>
     </row>
     <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="254"/>
-      <c r="B65" s="234"/>
+      <c r="A65" s="225"/>
+      <c r="B65" s="250"/>
       <c r="C65" s="76"/>
       <c r="D65" s="76"/>
       <c r="E65" s="76"/>
@@ -6678,10 +6674,10 @@
     </row>
     <row r="67" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" s="42" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -6720,79 +6716,111 @@
       <c r="K69" s="1"/>
     </row>
     <row r="70" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A70" s="229" t="s">
+      <c r="A70" s="245" t="s">
         <v>39</v>
       </c>
-      <c r="B70" s="230"/>
-      <c r="C70" s="231"/>
-      <c r="D70" s="227" t="s">
+      <c r="B70" s="246"/>
+      <c r="C70" s="247"/>
+      <c r="D70" s="243" t="s">
         <v>40</v>
       </c>
-      <c r="E70" s="227"/>
-      <c r="F70" s="227" t="s">
+      <c r="E70" s="243"/>
+      <c r="F70" s="243" t="s">
         <v>41</v>
       </c>
-      <c r="G70" s="227"/>
-      <c r="H70" s="227" t="s">
+      <c r="G70" s="243"/>
+      <c r="H70" s="243" t="s">
         <v>42</v>
       </c>
-      <c r="I70" s="228"/>
+      <c r="I70" s="244"/>
       <c r="J70" s="78" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K70" s="1"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="219" t="s">
+      <c r="A71" s="251" t="s">
         <v>43</v>
       </c>
-      <c r="B71" s="220"/>
-      <c r="C71" s="220"/>
-      <c r="D71" s="210" t="s">
+      <c r="B71" s="252"/>
+      <c r="C71" s="252"/>
+      <c r="D71" s="255" t="s">
         <v>44</v>
       </c>
-      <c r="E71" s="211"/>
-      <c r="F71" s="210" t="s">
+      <c r="E71" s="256"/>
+      <c r="F71" s="255" t="s">
         <v>44</v>
       </c>
-      <c r="G71" s="211"/>
-      <c r="H71" s="210" t="s">
+      <c r="G71" s="256"/>
+      <c r="H71" s="255" t="s">
         <v>44</v>
       </c>
-      <c r="I71" s="216"/>
+      <c r="I71" s="261"/>
       <c r="J71" s="79">
         <v>1</v>
       </c>
       <c r="K71" s="1"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="219"/>
-      <c r="B72" s="220"/>
-      <c r="C72" s="220"/>
-      <c r="D72" s="212"/>
-      <c r="E72" s="213"/>
-      <c r="F72" s="212"/>
-      <c r="G72" s="213"/>
-      <c r="H72" s="212"/>
-      <c r="I72" s="217"/>
+      <c r="A72" s="251"/>
+      <c r="B72" s="252"/>
+      <c r="C72" s="252"/>
+      <c r="D72" s="257"/>
+      <c r="E72" s="258"/>
+      <c r="F72" s="257"/>
+      <c r="G72" s="258"/>
+      <c r="H72" s="257"/>
+      <c r="I72" s="262"/>
       <c r="J72" s="44"/>
       <c r="K72" s="1"/>
     </row>
     <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="221"/>
-      <c r="B73" s="222"/>
-      <c r="C73" s="222"/>
-      <c r="D73" s="214"/>
-      <c r="E73" s="215"/>
-      <c r="F73" s="214"/>
-      <c r="G73" s="215"/>
-      <c r="H73" s="214"/>
-      <c r="I73" s="218"/>
+      <c r="A73" s="253"/>
+      <c r="B73" s="254"/>
+      <c r="C73" s="254"/>
+      <c r="D73" s="259"/>
+      <c r="E73" s="260"/>
+      <c r="F73" s="259"/>
+      <c r="G73" s="260"/>
+      <c r="H73" s="259"/>
+      <c r="I73" s="263"/>
       <c r="J73" s="80"/>
       <c r="K73" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="I15:I20"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="H9:H20"/>
+    <mergeCell ref="I9:I14"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K15"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="C9:C20"/>
+    <mergeCell ref="D9:D20"/>
+    <mergeCell ref="E9:E20"/>
+    <mergeCell ref="F9:F20"/>
+    <mergeCell ref="G9:G20"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="B57:K57"/>
     <mergeCell ref="G60:G61"/>
@@ -6809,38 +6837,6 @@
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="B9:B20"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K9:K15"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="C9:C20"/>
-    <mergeCell ref="D9:D20"/>
-    <mergeCell ref="E9:E20"/>
-    <mergeCell ref="F9:F20"/>
-    <mergeCell ref="G9:G20"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="I15:I20"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="H9:H20"/>
-    <mergeCell ref="I9:I14"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H73:I73"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6860,7 +6856,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>